<commit_message>
Question labels removed from set_row so they can wrap.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -1170,7 +1170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1">
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1">
+    <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
         <v>45</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="12.75" customHeight="1">
+    <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="12.75" customHeight="1">
+    <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="12.75" customHeight="1">
+    <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
         <v>48</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Updates to excel test 'complex 2' and 'complex 3'.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2908" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="166">
   <si>
     <t>gender. What is your gender?</t>
   </si>
@@ -158,6 +158,9 @@
     <t>q5_2. How likely are you to do each of the following in the next year? - Snowboarding</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>q5_3. How likely are you to do each of the following in the next year? - Kite boarding</t>
   </si>
   <si>
@@ -192,9 +195,6 @@
   </si>
   <si>
     <t>Don't know (it varies a lot)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>q9. For what reasons might you visit a sporting goods store in the future?</t>
@@ -2507,28 +2507,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>8255</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5">
-        <v>3952</v>
+        <v>17</v>
       </c>
       <c r="D13" s="6">
-        <v>4303</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5">
-        <v>3106</v>
+        <v>12</v>
       </c>
       <c r="F13" s="5">
-        <v>2245</v>
+        <v>9</v>
       </c>
       <c r="G13" s="5">
-        <v>1180</v>
-      </c>
-      <c r="H13" s="5">
-        <v>718</v>
+        <v>7</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="I13" s="6">
-        <v>829</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1">
@@ -2536,28 +2536,28 @@
         <v>37</v>
       </c>
       <c r="B14" s="7">
-        <v>685</v>
-      </c>
-      <c r="C14" s="8">
-        <v>341</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D14" s="9">
-        <v>344</v>
+        <v>1</v>
       </c>
       <c r="E14" s="8">
-        <v>240</v>
-      </c>
-      <c r="F14" s="8">
-        <v>176</v>
-      </c>
-      <c r="G14" s="8">
-        <v>124</v>
-      </c>
-      <c r="H14" s="8">
-        <v>67</v>
-      </c>
-      <c r="I14" s="9">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1">
@@ -2565,28 +2565,28 @@
         <v>38</v>
       </c>
       <c r="B15" s="11">
-        <v>1302</v>
+        <v>8</v>
       </c>
       <c r="C15" s="12">
-        <v>591</v>
+        <v>4</v>
       </c>
       <c r="D15" s="13">
-        <v>711</v>
+        <v>4</v>
       </c>
       <c r="E15" s="12">
-        <v>575</v>
+        <v>4</v>
       </c>
       <c r="F15" s="12">
-        <v>365</v>
-      </c>
-      <c r="G15" s="12">
-        <v>145</v>
-      </c>
-      <c r="H15" s="12">
-        <v>92</v>
-      </c>
-      <c r="I15" s="13">
-        <v>87</v>
+        <v>4</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1">
@@ -2594,57 +2594,57 @@
         <v>39</v>
       </c>
       <c r="B16" s="7">
-        <v>2819</v>
+        <v>7</v>
       </c>
       <c r="C16" s="8">
-        <v>1414</v>
+        <v>3</v>
       </c>
       <c r="D16" s="9">
-        <v>1405</v>
+        <v>4</v>
       </c>
       <c r="E16" s="8">
-        <v>1087</v>
+        <v>1</v>
       </c>
       <c r="F16" s="8">
-        <v>773</v>
+        <v>2</v>
       </c>
       <c r="G16" s="8">
-        <v>393</v>
-      </c>
-      <c r="H16" s="8">
-        <v>222</v>
+        <v>3</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="I16" s="9">
-        <v>296</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="11">
-        <v>68</v>
-      </c>
-      <c r="C17" s="12">
-        <v>44</v>
-      </c>
-      <c r="D17" s="13">
-        <v>24</v>
-      </c>
-      <c r="E17" s="12">
-        <v>24</v>
-      </c>
-      <c r="F17" s="12">
-        <v>23</v>
-      </c>
-      <c r="G17" s="12">
-        <v>8</v>
-      </c>
-      <c r="H17" s="12">
-        <v>4</v>
-      </c>
-      <c r="I17" s="13">
-        <v>8</v>
+      <c r="B17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1">
@@ -2652,28 +2652,28 @@
         <v>41</v>
       </c>
       <c r="B18" s="7">
-        <v>1714</v>
+        <v>8</v>
       </c>
       <c r="C18" s="8">
-        <v>775</v>
+        <v>5</v>
       </c>
       <c r="D18" s="9">
-        <v>939</v>
+        <v>3</v>
       </c>
       <c r="E18" s="8">
-        <v>621</v>
+        <v>4</v>
       </c>
       <c r="F18" s="8">
-        <v>475</v>
+        <v>1</v>
       </c>
       <c r="G18" s="8">
-        <v>268</v>
-      </c>
-      <c r="H18" s="8">
-        <v>161</v>
-      </c>
-      <c r="I18" s="9">
-        <v>152</v>
+        <v>3</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1">
@@ -2681,28 +2681,28 @@
         <v>42</v>
       </c>
       <c r="B19" s="11">
-        <v>193</v>
+        <v>2</v>
       </c>
       <c r="C19" s="12">
-        <v>116</v>
-      </c>
-      <c r="D19" s="13">
-        <v>77</v>
-      </c>
-      <c r="E19" s="12">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="F19" s="12">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="12">
-        <v>29</v>
-      </c>
-      <c r="H19" s="12">
-        <v>22</v>
-      </c>
-      <c r="I19" s="13">
-        <v>31</v>
+      <c r="H19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1">
@@ -2710,33 +2710,33 @@
         <v>43</v>
       </c>
       <c r="B20" s="17">
-        <v>1474</v>
+        <v>4</v>
       </c>
       <c r="C20" s="18">
-        <v>671</v>
+        <v>3</v>
       </c>
       <c r="D20" s="19">
-        <v>803</v>
+        <v>1</v>
       </c>
       <c r="E20" s="18">
-        <v>501</v>
+        <v>2</v>
       </c>
       <c r="F20" s="18">
-        <v>388</v>
+        <v>1</v>
       </c>
       <c r="G20" s="18">
-        <v>213</v>
-      </c>
-      <c r="H20" s="18">
-        <v>150</v>
-      </c>
-      <c r="I20" s="19">
-        <v>195</v>
+        <v>1</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2997,28 +2997,28 @@
         <v>11</v>
       </c>
       <c r="B31" s="4">
-        <v>8255</v>
+        <v>30</v>
       </c>
       <c r="C31" s="5">
-        <v>3952</v>
+        <v>17</v>
       </c>
       <c r="D31" s="6">
-        <v>4303</v>
+        <v>13</v>
       </c>
       <c r="E31" s="5">
-        <v>3106</v>
+        <v>12</v>
       </c>
       <c r="F31" s="5">
-        <v>2245</v>
+        <v>9</v>
       </c>
       <c r="G31" s="5">
-        <v>1180</v>
-      </c>
-      <c r="H31" s="5">
-        <v>718</v>
+        <v>7</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="I31" s="6">
-        <v>829</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1">
@@ -3026,28 +3026,28 @@
         <v>37</v>
       </c>
       <c r="B32" s="7">
-        <v>550</v>
-      </c>
-      <c r="C32" s="8">
-        <v>256</v>
+        <v>1</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D32" s="9">
-        <v>294</v>
-      </c>
-      <c r="E32" s="8">
-        <v>205</v>
-      </c>
-      <c r="F32" s="8">
-        <v>148</v>
+        <v>1</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="G32" s="8">
-        <v>85</v>
-      </c>
-      <c r="H32" s="8">
-        <v>51</v>
-      </c>
-      <c r="I32" s="9">
-        <v>55</v>
+        <v>1</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1">
@@ -3055,28 +3055,28 @@
         <v>38</v>
       </c>
       <c r="B33" s="11">
-        <v>848</v>
+        <v>6</v>
       </c>
       <c r="C33" s="12">
-        <v>382</v>
+        <v>5</v>
       </c>
       <c r="D33" s="13">
-        <v>466</v>
+        <v>1</v>
       </c>
       <c r="E33" s="12">
-        <v>375</v>
+        <v>3</v>
       </c>
       <c r="F33" s="12">
-        <v>225</v>
+        <v>2</v>
       </c>
       <c r="G33" s="12">
-        <v>110</v>
-      </c>
-      <c r="H33" s="12">
-        <v>56</v>
-      </c>
-      <c r="I33" s="13">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1">
@@ -3084,57 +3084,57 @@
         <v>39</v>
       </c>
       <c r="B34" s="7">
-        <v>1796</v>
+        <v>8</v>
       </c>
       <c r="C34" s="8">
-        <v>881</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9">
-        <v>915</v>
+        <v>7</v>
       </c>
       <c r="E34" s="8">
-        <v>656</v>
+        <v>1</v>
       </c>
       <c r="F34" s="8">
-        <v>509</v>
+        <v>2</v>
       </c>
       <c r="G34" s="8">
-        <v>269</v>
-      </c>
-      <c r="H34" s="8">
-        <v>139</v>
+        <v>4</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="I34" s="9">
-        <v>190</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="11">
-        <v>71</v>
-      </c>
-      <c r="C35" s="12">
-        <v>42</v>
-      </c>
-      <c r="D35" s="13">
-        <v>29</v>
-      </c>
-      <c r="E35" s="12">
-        <v>20</v>
-      </c>
-      <c r="F35" s="12">
-        <v>22</v>
-      </c>
-      <c r="G35" s="12">
-        <v>11</v>
-      </c>
-      <c r="H35" s="12">
-        <v>9</v>
-      </c>
-      <c r="I35" s="13">
-        <v>7</v>
+      <c r="B35" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1">
@@ -3142,28 +3142,28 @@
         <v>41</v>
       </c>
       <c r="B36" s="7">
-        <v>1800</v>
+        <v>6</v>
       </c>
       <c r="C36" s="8">
-        <v>876</v>
+        <v>5</v>
       </c>
       <c r="D36" s="9">
-        <v>924</v>
+        <v>1</v>
       </c>
       <c r="E36" s="8">
-        <v>681</v>
+        <v>4</v>
       </c>
       <c r="F36" s="8">
-        <v>489</v>
-      </c>
-      <c r="G36" s="8">
-        <v>262</v>
-      </c>
-      <c r="H36" s="8">
-        <v>165</v>
-      </c>
-      <c r="I36" s="9">
-        <v>156</v>
+        <v>2</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1">
@@ -3171,28 +3171,28 @@
         <v>42</v>
       </c>
       <c r="B37" s="11">
-        <v>635</v>
+        <v>2</v>
       </c>
       <c r="C37" s="12">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="D37" s="13">
-        <v>307</v>
+        <v>1</v>
       </c>
       <c r="E37" s="12">
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="F37" s="12">
-        <v>166</v>
-      </c>
-      <c r="G37" s="12">
-        <v>75</v>
-      </c>
-      <c r="H37" s="12">
-        <v>55</v>
-      </c>
-      <c r="I37" s="13">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1">
@@ -3200,33 +3200,33 @@
         <v>43</v>
       </c>
       <c r="B38" s="17">
-        <v>2555</v>
+        <v>7</v>
       </c>
       <c r="C38" s="18">
-        <v>1187</v>
+        <v>5</v>
       </c>
       <c r="D38" s="19">
-        <v>1368</v>
+        <v>2</v>
       </c>
       <c r="E38" s="18">
-        <v>925</v>
+        <v>3</v>
       </c>
       <c r="F38" s="18">
-        <v>686</v>
+        <v>2</v>
       </c>
       <c r="G38" s="18">
-        <v>368</v>
-      </c>
-      <c r="H38" s="18">
-        <v>243</v>
-      </c>
-      <c r="I38" s="19">
-        <v>290</v>
+        <v>1</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3783,7 +3783,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="7">
         <v>949</v>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="11">
         <v>216</v>
@@ -3883,7 +3883,7 @@
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="7">
         <v>595</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="11">
         <v>970</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="7">
         <v>1235</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="11">
         <v>283</v>
@@ -3999,7 +3999,7 @@
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="17">
         <v>49</v>
@@ -4023,7 +4023,7 @@
         <v>3</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding column_width_specific attribute to have custom column widths, whether in chain area or not.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -817,6 +817,24 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -829,15 +847,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,15 +854,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1173,8 +1173,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -1289,31 +1297,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>1366</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>730</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>636</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>618</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>340</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>198</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <v>102</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <v>92</v>
       </c>
     </row>
@@ -1321,57 +1329,57 @@
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>1721</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>878</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>843</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="12">
         <v>720</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>455</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <v>241</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="12">
         <v>145</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="13">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>649</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>329</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>320</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>271</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>149</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>101</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>55</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>63</v>
       </c>
     </row>
@@ -1379,57 +1387,57 @@
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="11">
         <v>458</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>258</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>200</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="12">
         <v>212</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>110</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="12">
         <v>69</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="12">
         <v>27</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="13">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>428</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>176</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>252</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>157</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>102</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>74</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <v>43</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <v>43</v>
       </c>
     </row>
@@ -1437,57 +1445,57 @@
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="11">
         <v>492</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="12">
         <v>205</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <v>287</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="12">
         <v>171</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="12">
         <v>135</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="12">
         <v>63</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="12">
         <v>48</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="13">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="14">
         <v>53</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="15">
         <v>17</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="16">
         <v>36</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="15">
         <v>21</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="15">
         <v>13</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="15">
         <v>7</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="15">
         <v>5</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="16">
         <v>6</v>
       </c>
     </row>
@@ -1515,7 +1523,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -1630,31 +1645,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="18">
         <v>5147</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="19">
         <v>2458</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="20">
         <v>2689</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="19">
         <v>2023</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="19">
         <v>1304</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="19">
         <v>739</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="19">
         <v>432</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="20">
         <v>532</v>
       </c>
     </row>
@@ -1662,28 +1677,28 @@
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="14">
         <v>419</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="15">
         <v>155</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="16">
         <v>264</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="15">
         <v>155</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="15">
         <v>97</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="15">
         <v>58</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="15">
         <v>42</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="16">
         <v>59</v>
       </c>
     </row>
@@ -1711,7 +1726,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -1826,31 +1848,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="18">
         <v>4801</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="19">
         <v>2287</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="20">
         <v>2514</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="19">
         <v>1981</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="19">
         <v>1322</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="19">
         <v>654</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="19">
         <v>360</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="20">
         <v>381</v>
       </c>
     </row>
@@ -1858,57 +1880,57 @@
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>7214</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>3516</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>3698</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="12">
         <v>2752</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>1989</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <v>1019</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="12">
         <v>602</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="13">
         <v>704</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="18">
         <v>576</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="19">
         <v>248</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="20">
         <v>328</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="19">
         <v>202</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="19">
         <v>172</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="19">
         <v>87</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="19">
         <v>61</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="20">
         <v>45</v>
       </c>
     </row>
@@ -1916,57 +1938,57 @@
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="11">
         <v>190</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>86</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>104</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="12">
         <v>80</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>54</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="12">
         <v>25</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="12">
         <v>8</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="13">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="18">
         <v>159</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="19">
         <v>81</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="20">
         <v>78</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="19">
         <v>82</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="19">
         <v>33</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="19">
         <v>25</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="19">
         <v>4</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="20">
         <v>13</v>
       </c>
     </row>
@@ -1974,57 +1996,57 @@
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="11">
         <v>1674</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="12">
         <v>877</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <v>797</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="12">
         <v>709</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="12">
         <v>454</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="12">
         <v>222</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="12">
         <v>125</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="13">
         <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="18">
         <v>251</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="19">
         <v>126</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="20">
         <v>125</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="19">
         <v>93</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="19">
         <v>63</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="19">
         <v>54</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="19">
         <v>16</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="20">
         <v>19</v>
       </c>
     </row>
@@ -2032,28 +2054,28 @@
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="14">
         <v>232</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="15">
         <v>116</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="16">
         <v>116</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="15">
         <v>68</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="15">
         <v>60</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="15">
         <v>37</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="15">
         <v>26</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="16">
         <v>37</v>
       </c>
     </row>
@@ -2081,7 +2103,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -2196,31 +2225,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="21">
         <v>5360</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="22">
         <v>2305</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="23">
         <v>3055</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="22">
         <v>1959</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="22">
         <v>1407</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="22">
         <v>787</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="22">
         <v>507</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="23">
         <v>586</v>
       </c>
     </row>
@@ -2248,7 +2277,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -2363,31 +2399,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="18">
         <v>700</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="19">
         <v>314</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="20">
         <v>386</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="19">
         <v>307</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="19">
         <v>183</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="19">
         <v>90</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="19">
         <v>53</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="20">
         <v>47</v>
       </c>
     </row>
@@ -2395,57 +2431,57 @@
       <c r="A7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>2598</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>1452</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>1146</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="12">
         <v>1010</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>722</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <v>357</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="12">
         <v>201</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="13">
         <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="18">
         <v>124</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="19">
         <v>67</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="20">
         <v>57</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="19">
         <v>35</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="19">
         <v>41</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="19">
         <v>28</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="19">
         <v>9</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="20">
         <v>10</v>
       </c>
     </row>
@@ -2453,57 +2489,57 @@
       <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="11">
         <v>2472</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>1032</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>1440</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="12">
         <v>943</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>680</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="12">
         <v>351</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="12">
         <v>225</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="13">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="18">
         <v>200</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="19">
         <v>120</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="20">
         <v>80</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="19">
         <v>59</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="19">
         <v>48</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="19">
         <v>32</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="19">
         <v>19</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="20">
         <v>36</v>
       </c>
     </row>
@@ -2511,28 +2547,28 @@
       <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="14">
         <v>1798</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="15">
         <v>781</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="16">
         <v>1017</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="15">
         <v>628</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="15">
         <v>484</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="15">
         <v>252</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>176</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="16">
         <v>216</v>
       </c>
     </row>
@@ -2608,31 +2644,31 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="18">
         <v>8</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="19">
         <v>4</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="20">
         <v>4</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="19">
         <v>4</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="19">
         <v>4</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2640,57 +2676,57 @@
       <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="11">
         <v>7</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="12">
         <v>3</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="13">
         <v>4</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="12">
         <v>1</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="12">
         <v>2</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="12">
         <v>3</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2698,57 +2734,57 @@
       <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="11">
         <v>8</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="12">
         <v>5</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="13">
         <v>3</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="12">
         <v>4</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="12">
         <v>1</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="12">
         <v>3</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="18">
         <v>2</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="19">
         <v>2</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="19">
         <v>1</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2756,28 +2792,28 @@
       <c r="A20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="14">
         <v>4</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="15">
         <v>3</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="16">
         <v>1</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="15">
         <v>2</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="15">
         <v>1</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="15">
         <v>1</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="16" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2853,31 +2889,31 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="18">
         <v>1245</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="19">
         <v>575</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="20">
         <v>670</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="19">
         <v>554</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="19">
         <v>329</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="19">
         <v>157</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="19">
         <v>89</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="20">
         <v>80</v>
       </c>
     </row>
@@ -2885,57 +2921,57 @@
       <c r="A25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="11">
         <v>2702</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="12">
         <v>1319</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="13">
         <v>1383</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="12">
         <v>1002</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="12">
         <v>749</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="12">
         <v>394</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="12">
         <v>216</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="13">
         <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="18">
         <v>66</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="19">
         <v>40</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="20">
         <v>26</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="19">
         <v>22</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="19">
         <v>21</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="19">
         <v>10</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="19">
         <v>6</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="20">
         <v>6</v>
       </c>
     </row>
@@ -2943,57 +2979,57 @@
       <c r="A27" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="11">
         <v>1710</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="12">
         <v>820</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="13">
         <v>890</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="12">
         <v>629</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="12">
         <v>487</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="12">
         <v>256</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="12">
         <v>153</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="13">
         <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="18">
         <v>309</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="19">
         <v>164</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="20">
         <v>145</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="19">
         <v>101</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="19">
         <v>67</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="19">
         <v>47</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="19">
         <v>34</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="20">
         <v>46</v>
       </c>
     </row>
@@ -3001,28 +3037,28 @@
       <c r="A29" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="14">
         <v>1611</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="15">
         <v>744</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="16">
         <v>867</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="15">
         <v>583</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="15">
         <v>425</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="15">
         <v>214</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="15">
         <v>160</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="16">
         <v>197</v>
       </c>
     </row>
@@ -3098,31 +3134,31 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="18">
         <v>6</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="19">
         <v>5</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="20">
         <v>1</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="19">
         <v>3</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="19">
         <v>2</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="19">
         <v>1</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3130,57 +3166,57 @@
       <c r="A34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="11">
         <v>8</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="12">
         <v>1</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="13">
         <v>7</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="12">
         <v>1</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="12">
         <v>2</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="12">
         <v>4</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3188,57 +3224,57 @@
       <c r="A36" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="11">
         <v>6</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="12">
         <v>5</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="13">
         <v>1</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="12">
         <v>4</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="12">
         <v>2</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="18">
         <v>2</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="19">
         <v>1</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="20">
         <v>1</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="19">
         <v>1</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="19">
         <v>1</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3246,28 +3282,28 @@
       <c r="A38" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="21">
+      <c r="B38" s="14">
         <v>7</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="15">
         <v>5</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="16">
         <v>2</v>
       </c>
-      <c r="E38" s="22">
+      <c r="E38" s="15">
         <v>3</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="15">
         <v>2</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="15">
         <v>1</v>
       </c>
-      <c r="H38" s="22" t="s">
+      <c r="H38" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I38" s="23" t="s">
+      <c r="I38" s="16" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3343,31 +3379,31 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="18">
         <v>1127</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="19">
         <v>497</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="20">
         <v>630</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="19">
         <v>501</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="19">
         <v>307</v>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="19">
         <v>135</v>
       </c>
-      <c r="H42" s="13">
+      <c r="H42" s="19">
         <v>77</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="20">
         <v>78</v>
       </c>
     </row>
@@ -3375,57 +3411,57 @@
       <c r="A43" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="11">
         <v>2193</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43" s="12">
         <v>1149</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="13">
         <v>1044</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E43" s="12">
         <v>816</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="12">
         <v>603</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="12">
         <v>321</v>
       </c>
-      <c r="H43" s="16">
+      <c r="H43" s="12">
         <v>178</v>
       </c>
-      <c r="I43" s="17">
+      <c r="I43" s="13">
         <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="18">
         <v>34</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="19">
         <v>22</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="20">
         <v>12</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="19">
         <v>14</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="19">
         <v>12</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="19">
         <v>4</v>
       </c>
-      <c r="H44" s="13">
+      <c r="H44" s="19">
         <v>1</v>
       </c>
-      <c r="I44" s="14">
+      <c r="I44" s="20">
         <v>3</v>
       </c>
     </row>
@@ -3433,57 +3469,57 @@
       <c r="A45" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="11">
         <v>225</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="12">
         <v>112</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="13">
         <v>113</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="12">
         <v>78</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="12">
         <v>56</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="12">
         <v>48</v>
       </c>
-      <c r="H45" s="16">
+      <c r="H45" s="12">
         <v>16</v>
       </c>
-      <c r="I45" s="17">
+      <c r="I45" s="13">
         <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="18">
         <v>366</v>
       </c>
-      <c r="C46" s="13">
+      <c r="C46" s="19">
         <v>176</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="20">
         <v>190</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="19">
         <v>109</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="19">
         <v>87</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="19">
         <v>52</v>
       </c>
-      <c r="H46" s="13">
+      <c r="H46" s="19">
         <v>41</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="20">
         <v>64</v>
       </c>
     </row>
@@ -3491,28 +3527,28 @@
       <c r="A47" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="21">
+      <c r="B47" s="14">
         <v>1562</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="15">
         <v>745</v>
       </c>
-      <c r="D47" s="23">
+      <c r="D47" s="16">
         <v>817</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="15">
         <v>538</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F47" s="15">
         <v>394</v>
       </c>
-      <c r="G47" s="22">
+      <c r="G47" s="15">
         <v>227</v>
       </c>
-      <c r="H47" s="22">
+      <c r="H47" s="15">
         <v>166</v>
       </c>
-      <c r="I47" s="23">
+      <c r="I47" s="16">
         <v>206</v>
       </c>
     </row>
@@ -3588,31 +3624,31 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51" s="18">
         <v>678</v>
       </c>
-      <c r="C51" s="13">
+      <c r="C51" s="19">
         <v>332</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="20">
         <v>346</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="19">
         <v>294</v>
       </c>
-      <c r="F51" s="13">
+      <c r="F51" s="19">
         <v>185</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="19">
         <v>96</v>
       </c>
-      <c r="H51" s="13">
+      <c r="H51" s="19">
         <v>45</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="20">
         <v>40</v>
       </c>
     </row>
@@ -3620,57 +3656,57 @@
       <c r="A52" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="11">
         <v>2516</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52" s="12">
         <v>1309</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="13">
         <v>1207</v>
       </c>
-      <c r="E52" s="16">
+      <c r="E52" s="12">
         <v>1000</v>
       </c>
-      <c r="F52" s="16">
+      <c r="F52" s="12">
         <v>695</v>
       </c>
-      <c r="G52" s="16">
+      <c r="G52" s="12">
         <v>344</v>
       </c>
-      <c r="H52" s="16">
+      <c r="H52" s="12">
         <v>187</v>
       </c>
-      <c r="I52" s="17">
+      <c r="I52" s="13">
         <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B53" s="18">
         <v>104</v>
       </c>
-      <c r="C53" s="13">
+      <c r="C53" s="19">
         <v>53</v>
       </c>
-      <c r="D53" s="14">
+      <c r="D53" s="20">
         <v>51</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E53" s="19">
         <v>30</v>
       </c>
-      <c r="F53" s="13">
+      <c r="F53" s="19">
         <v>35</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="19">
         <v>15</v>
       </c>
-      <c r="H53" s="13">
+      <c r="H53" s="19">
         <v>8</v>
       </c>
-      <c r="I53" s="14">
+      <c r="I53" s="20">
         <v>14</v>
       </c>
     </row>
@@ -3678,57 +3714,57 @@
       <c r="A54" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="11">
         <v>2294</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54" s="12">
         <v>1002</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="13">
         <v>1292</v>
       </c>
-      <c r="E54" s="16">
+      <c r="E54" s="12">
         <v>863</v>
       </c>
-      <c r="F54" s="16">
+      <c r="F54" s="12">
         <v>653</v>
       </c>
-      <c r="G54" s="16">
+      <c r="G54" s="12">
         <v>330</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H54" s="12">
         <v>197</v>
       </c>
-      <c r="I54" s="17">
+      <c r="I54" s="13">
         <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B55" s="12">
+      <c r="B55" s="18">
         <v>211</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="19">
         <v>125</v>
       </c>
-      <c r="D55" s="14">
+      <c r="D55" s="20">
         <v>86</v>
       </c>
-      <c r="E55" s="13">
+      <c r="E55" s="19">
         <v>61</v>
       </c>
-      <c r="F55" s="13">
+      <c r="F55" s="19">
         <v>51</v>
       </c>
-      <c r="G55" s="13">
+      <c r="G55" s="19">
         <v>31</v>
       </c>
-      <c r="H55" s="13">
+      <c r="H55" s="19">
         <v>25</v>
       </c>
-      <c r="I55" s="14">
+      <c r="I55" s="20">
         <v>39</v>
       </c>
     </row>
@@ -3736,28 +3772,28 @@
       <c r="A56" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="21">
+      <c r="B56" s="14">
         <v>2015</v>
       </c>
-      <c r="C56" s="22">
+      <c r="C56" s="15">
         <v>926</v>
       </c>
-      <c r="D56" s="23">
+      <c r="D56" s="16">
         <v>1089</v>
       </c>
-      <c r="E56" s="22">
+      <c r="E56" s="15">
         <v>712</v>
       </c>
-      <c r="F56" s="22">
+      <c r="F56" s="15">
         <v>518</v>
       </c>
-      <c r="G56" s="22">
+      <c r="G56" s="15">
         <v>289</v>
       </c>
-      <c r="H56" s="22">
+      <c r="H56" s="15">
         <v>200</v>
       </c>
-      <c r="I56" s="23">
+      <c r="I56" s="16">
         <v>242</v>
       </c>
     </row>
@@ -3785,7 +3821,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -3900,31 +3943,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="18">
         <v>216</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="19">
         <v>112</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="20">
         <v>104</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="19">
         <v>97</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="19">
         <v>55</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="19">
         <v>25</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="19">
         <v>18</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="20">
         <v>16</v>
       </c>
     </row>
@@ -3932,57 +3975,57 @@
       <c r="A7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>595</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>293</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>302</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="12">
         <v>263</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>170</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <v>72</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="12">
         <v>31</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="13">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="18">
         <v>970</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="19">
         <v>507</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="20">
         <v>463</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="19">
         <v>413</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="19">
         <v>250</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="19">
         <v>139</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="19">
         <v>70</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="20">
         <v>82</v>
       </c>
     </row>
@@ -3990,57 +4033,57 @@
       <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="11">
         <v>1235</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>636</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>599</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="12">
         <v>501</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>354</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="12">
         <v>162</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="12">
         <v>90</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="13">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="18">
         <v>283</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="19">
         <v>165</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="20">
         <v>118</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="19">
         <v>128</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="19">
         <v>78</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="19">
         <v>33</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="19">
         <v>14</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="20">
         <v>24</v>
       </c>
     </row>
@@ -4048,28 +4091,28 @@
       <c r="A11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="14">
         <v>49</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="15">
         <v>26</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="16">
         <v>23</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="15">
         <v>15</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="15">
         <v>19</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="15">
         <v>10</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>3</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="16" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4097,7 +4140,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1">
@@ -4212,31 +4262,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="18">
         <v>1603</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="19">
         <v>785</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="20">
         <v>818</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="19">
         <v>598</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="19">
         <v>448</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="19">
         <v>233</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="19">
         <v>140</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="20">
         <v>151</v>
       </c>
     </row>
@@ -4244,57 +4294,57 @@
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>861</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>379</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>482</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="12">
         <v>354</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>245</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <v>108</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="12">
         <v>69</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="13">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="18">
         <v>2177</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="19">
         <v>883</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="20">
         <v>1294</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="19">
         <v>895</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="19">
         <v>593</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="19">
         <v>287</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="19">
         <v>173</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="20">
         <v>180</v>
       </c>
     </row>
@@ -4302,57 +4352,57 @@
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="11">
         <v>367</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>172</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>195</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="12">
         <v>159</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>102</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="12">
         <v>39</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="12">
         <v>19</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="13">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="18">
         <v>1358</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="19">
         <v>689</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="20">
         <v>669</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="19">
         <v>495</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="19">
         <v>391</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="19">
         <v>201</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="19">
         <v>106</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="20">
         <v>141</v>
       </c>
     </row>
@@ -4360,28 +4410,28 @@
       <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="14">
         <v>2883</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="15">
         <v>1463</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="16">
         <v>1420</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="15">
         <v>1003</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="15">
         <v>740</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="15">
         <v>424</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>281</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="16">
         <v>369</v>
       </c>
     </row>
@@ -4406,8 +4456,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.75" customHeight="1">

</xml_diff>

<commit_message>
Only setting rows when we do not need text wrap or text size isn't larger than row height.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -4261,7 +4261,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:9">
       <c r="A6" s="17" t="s">
         <v>60</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+    <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
freeze loc offset bugfix.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -1153,8 +1153,8 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -1502,8 +1502,8 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -1705,8 +1705,8 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2082,8 +2082,8 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2256,8 +2256,8 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -3800,8 +3800,8 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -4119,8 +4119,8 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>

</xml_diff>

<commit_message>
Checks on Excel xbreak border limits, to stop question label merging when neighbours have identical labels.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="164">
   <si>
     <t>gender. What is your gender?</t>
   </si>
@@ -1144,7 +1144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -1164,10 +1164,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1176,14 +1177,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1192,22 +1197,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1219,8 +1230,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1234,22 +1247,28 @@
         <v>1561</v>
       </c>
       <c r="E4" s="5">
+        <v>1438</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1561</v>
+      </c>
+      <c r="G4" s="5">
         <v>1200</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>767</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>435</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>270</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1263,22 +1282,28 @@
         <v>552</v>
       </c>
       <c r="E5" s="9">
+        <v>575</v>
+      </c>
+      <c r="F5" s="10">
+        <v>552</v>
+      </c>
+      <c r="G5" s="9">
         <v>480</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>274</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>166</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>99</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1292,22 +1317,28 @@
         <v>636</v>
       </c>
       <c r="E6" s="12">
+        <v>730</v>
+      </c>
+      <c r="F6" s="13">
+        <v>636</v>
+      </c>
+      <c r="G6" s="12">
         <v>618</v>
       </c>
-      <c r="F6" s="12">
+      <c r="H6" s="12">
         <v>340</v>
       </c>
-      <c r="G6" s="12">
+      <c r="I6" s="12">
         <v>198</v>
       </c>
-      <c r="H6" s="12">
+      <c r="J6" s="12">
         <v>102</v>
       </c>
-      <c r="I6" s="13">
+      <c r="K6" s="13">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1321,22 +1352,28 @@
         <v>843</v>
       </c>
       <c r="E7" s="12">
+        <v>878</v>
+      </c>
+      <c r="F7" s="13">
+        <v>843</v>
+      </c>
+      <c r="G7" s="12">
         <v>720</v>
       </c>
-      <c r="F7" s="12">
+      <c r="H7" s="12">
         <v>455</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>241</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>145</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1350,22 +1387,28 @@
         <v>320</v>
       </c>
       <c r="E8" s="12">
+        <v>329</v>
+      </c>
+      <c r="F8" s="13">
+        <v>320</v>
+      </c>
+      <c r="G8" s="12">
         <v>271</v>
       </c>
-      <c r="F8" s="12">
+      <c r="H8" s="12">
         <v>149</v>
       </c>
-      <c r="G8" s="12">
+      <c r="I8" s="12">
         <v>101</v>
       </c>
-      <c r="H8" s="12">
+      <c r="J8" s="12">
         <v>55</v>
       </c>
-      <c r="I8" s="13">
+      <c r="K8" s="13">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1379,22 +1422,28 @@
         <v>200</v>
       </c>
       <c r="E9" s="12">
+        <v>258</v>
+      </c>
+      <c r="F9" s="13">
+        <v>200</v>
+      </c>
+      <c r="G9" s="12">
         <v>212</v>
       </c>
-      <c r="F9" s="12">
+      <c r="H9" s="12">
         <v>110</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>69</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>27</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1408,22 +1457,28 @@
         <v>252</v>
       </c>
       <c r="E10" s="12">
+        <v>176</v>
+      </c>
+      <c r="F10" s="13">
+        <v>252</v>
+      </c>
+      <c r="G10" s="12">
         <v>157</v>
       </c>
-      <c r="F10" s="12">
+      <c r="H10" s="12">
         <v>102</v>
       </c>
-      <c r="G10" s="12">
+      <c r="I10" s="12">
         <v>74</v>
       </c>
-      <c r="H10" s="12">
+      <c r="J10" s="12">
         <v>43</v>
       </c>
-      <c r="I10" s="13">
+      <c r="K10" s="13">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1437,22 +1492,28 @@
         <v>287</v>
       </c>
       <c r="E11" s="12">
+        <v>205</v>
+      </c>
+      <c r="F11" s="13">
+        <v>287</v>
+      </c>
+      <c r="G11" s="12">
         <v>171</v>
       </c>
-      <c r="F11" s="12">
+      <c r="H11" s="12">
         <v>135</v>
       </c>
-      <c r="G11" s="12">
+      <c r="I11" s="12">
         <v>63</v>
       </c>
-      <c r="H11" s="12">
+      <c r="J11" s="12">
         <v>48</v>
       </c>
-      <c r="I11" s="13">
+      <c r="K11" s="13">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1466,25 +1527,32 @@
         <v>36</v>
       </c>
       <c r="E12" s="15">
+        <v>17</v>
+      </c>
+      <c r="F12" s="16">
+        <v>36</v>
+      </c>
+      <c r="G12" s="15">
         <v>21</v>
       </c>
-      <c r="F12" s="15">
+      <c r="H12" s="15">
         <v>13</v>
       </c>
-      <c r="G12" s="15">
+      <c r="I12" s="15">
         <v>7</v>
       </c>
-      <c r="H12" s="15">
+      <c r="J12" s="15">
         <v>5</v>
       </c>
-      <c r="I12" s="16">
+      <c r="K12" s="16">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1493,7 +1561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -1513,9 +1581,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1524,14 +1594,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1540,22 +1614,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1567,8 +1647,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1582,22 +1664,28 @@
         <v>3309</v>
       </c>
       <c r="E4" s="5">
+        <v>2998</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3309</v>
+      </c>
+      <c r="G4" s="5">
         <v>2465</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>1618</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>903</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>538</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -1611,22 +1699,28 @@
         <v>356</v>
       </c>
       <c r="E5" s="9">
+        <v>385</v>
+      </c>
+      <c r="F5" s="10">
+        <v>356</v>
+      </c>
+      <c r="G5" s="9">
         <v>287</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>217</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>106</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>64</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>20</v>
       </c>
@@ -1640,22 +1734,28 @@
         <v>2689</v>
       </c>
       <c r="E6" s="19">
+        <v>2458</v>
+      </c>
+      <c r="F6" s="20">
+        <v>2689</v>
+      </c>
+      <c r="G6" s="19">
         <v>2023</v>
       </c>
-      <c r="F6" s="19">
+      <c r="H6" s="19">
         <v>1304</v>
       </c>
-      <c r="G6" s="19">
+      <c r="I6" s="19">
         <v>739</v>
       </c>
-      <c r="H6" s="19">
+      <c r="J6" s="19">
         <v>432</v>
       </c>
-      <c r="I6" s="20">
+      <c r="K6" s="20">
         <v>532</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -1671,23 +1771,30 @@
       <c r="E7" s="15">
         <v>155</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="16">
+        <v>264</v>
+      </c>
+      <c r="G7" s="15">
+        <v>155</v>
+      </c>
+      <c r="H7" s="15">
         <v>97</v>
       </c>
-      <c r="G7" s="15">
+      <c r="I7" s="15">
         <v>58</v>
       </c>
-      <c r="H7" s="15">
+      <c r="J7" s="15">
         <v>42</v>
       </c>
-      <c r="I7" s="16">
+      <c r="K7" s="16">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1696,7 +1803,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -1716,9 +1823,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1727,14 +1836,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1743,22 +1856,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1770,8 +1889,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1785,22 +1906,28 @@
         <v>4303</v>
       </c>
       <c r="E4" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G4" s="5">
         <v>3106</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>2245</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>1180</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>718</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -1814,22 +1941,28 @@
         <v>2982</v>
       </c>
       <c r="E5" s="9">
+        <v>2772</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2982</v>
+      </c>
+      <c r="G5" s="9">
         <v>2269</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>1607</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>805</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>475</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>473</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
@@ -1843,22 +1976,28 @@
         <v>2514</v>
       </c>
       <c r="E6" s="19">
+        <v>2287</v>
+      </c>
+      <c r="F6" s="20">
+        <v>2514</v>
+      </c>
+      <c r="G6" s="19">
         <v>1981</v>
       </c>
-      <c r="F6" s="19">
+      <c r="H6" s="19">
         <v>1322</v>
       </c>
-      <c r="G6" s="19">
+      <c r="I6" s="19">
         <v>654</v>
       </c>
-      <c r="H6" s="19">
+      <c r="J6" s="19">
         <v>360</v>
       </c>
-      <c r="I6" s="20">
+      <c r="K6" s="20">
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
@@ -1872,22 +2011,28 @@
         <v>3698</v>
       </c>
       <c r="E7" s="12">
+        <v>3516</v>
+      </c>
+      <c r="F7" s="13">
+        <v>3698</v>
+      </c>
+      <c r="G7" s="12">
         <v>2752</v>
       </c>
-      <c r="F7" s="12">
+      <c r="H7" s="12">
         <v>1989</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>1019</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>602</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>704</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
@@ -1901,22 +2046,28 @@
         <v>328</v>
       </c>
       <c r="E8" s="19">
+        <v>248</v>
+      </c>
+      <c r="F8" s="20">
+        <v>328</v>
+      </c>
+      <c r="G8" s="19">
         <v>202</v>
       </c>
-      <c r="F8" s="19">
+      <c r="H8" s="19">
         <v>172</v>
       </c>
-      <c r="G8" s="19">
+      <c r="I8" s="19">
         <v>87</v>
       </c>
-      <c r="H8" s="19">
+      <c r="J8" s="19">
         <v>61</v>
       </c>
-      <c r="I8" s="20">
+      <c r="K8" s="20">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -1930,22 +2081,28 @@
         <v>104</v>
       </c>
       <c r="E9" s="12">
+        <v>86</v>
+      </c>
+      <c r="F9" s="13">
+        <v>104</v>
+      </c>
+      <c r="G9" s="12">
         <v>80</v>
       </c>
-      <c r="F9" s="12">
+      <c r="H9" s="12">
         <v>54</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>25</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>8</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>28</v>
       </c>
@@ -1959,22 +2116,28 @@
         <v>78</v>
       </c>
       <c r="E10" s="19">
+        <v>81</v>
+      </c>
+      <c r="F10" s="20">
+        <v>78</v>
+      </c>
+      <c r="G10" s="19">
         <v>82</v>
       </c>
-      <c r="F10" s="19">
+      <c r="H10" s="19">
         <v>33</v>
       </c>
-      <c r="G10" s="19">
+      <c r="I10" s="19">
         <v>25</v>
       </c>
-      <c r="H10" s="19">
+      <c r="J10" s="19">
         <v>4</v>
       </c>
-      <c r="I10" s="20">
+      <c r="K10" s="20">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -1988,22 +2151,28 @@
         <v>797</v>
       </c>
       <c r="E11" s="12">
+        <v>877</v>
+      </c>
+      <c r="F11" s="13">
+        <v>797</v>
+      </c>
+      <c r="G11" s="12">
         <v>709</v>
       </c>
-      <c r="F11" s="12">
+      <c r="H11" s="12">
         <v>454</v>
       </c>
-      <c r="G11" s="12">
+      <c r="I11" s="12">
         <v>222</v>
       </c>
-      <c r="H11" s="12">
+      <c r="J11" s="12">
         <v>125</v>
       </c>
-      <c r="I11" s="13">
+      <c r="K11" s="13">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>30</v>
       </c>
@@ -2017,22 +2186,28 @@
         <v>125</v>
       </c>
       <c r="E12" s="19">
+        <v>126</v>
+      </c>
+      <c r="F12" s="20">
+        <v>125</v>
+      </c>
+      <c r="G12" s="19">
         <v>93</v>
       </c>
-      <c r="F12" s="19">
+      <c r="H12" s="19">
         <v>63</v>
       </c>
-      <c r="G12" s="19">
+      <c r="I12" s="19">
         <v>54</v>
       </c>
-      <c r="H12" s="19">
+      <c r="J12" s="19">
         <v>16</v>
       </c>
-      <c r="I12" s="20">
+      <c r="K12" s="20">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -2046,25 +2221,32 @@
         <v>116</v>
       </c>
       <c r="E13" s="15">
+        <v>116</v>
+      </c>
+      <c r="F13" s="16">
+        <v>116</v>
+      </c>
+      <c r="G13" s="15">
         <v>68</v>
       </c>
-      <c r="F13" s="15">
+      <c r="H13" s="15">
         <v>60</v>
       </c>
-      <c r="G13" s="15">
+      <c r="I13" s="15">
         <v>37</v>
       </c>
-      <c r="H13" s="15">
+      <c r="J13" s="15">
         <v>26</v>
       </c>
-      <c r="I13" s="16">
+      <c r="K13" s="16">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2073,7 +2255,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -2093,9 +2275,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2104,14 +2288,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -2120,22 +2308,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -2147,8 +2341,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2162,22 +2358,28 @@
         <v>4303</v>
       </c>
       <c r="E4" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G4" s="5">
         <v>3106</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>2245</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>1180</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>718</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
@@ -2191,22 +2393,28 @@
         <v>1248</v>
       </c>
       <c r="E5" s="9">
+        <v>1647</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1248</v>
+      </c>
+      <c r="G5" s="9">
         <v>1147</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>838</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>393</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>211</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
@@ -2220,25 +2428,32 @@
         <v>3055</v>
       </c>
       <c r="E6" s="15">
+        <v>2305</v>
+      </c>
+      <c r="F6" s="16">
+        <v>3055</v>
+      </c>
+      <c r="G6" s="15">
         <v>1959</v>
       </c>
-      <c r="F6" s="15">
+      <c r="H6" s="15">
         <v>1407</v>
       </c>
-      <c r="G6" s="15">
+      <c r="I6" s="15">
         <v>787</v>
       </c>
-      <c r="H6" s="15">
+      <c r="J6" s="15">
         <v>507</v>
       </c>
-      <c r="I6" s="16">
+      <c r="K6" s="16">
         <v>586</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2247,7 +2462,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -2267,9 +2482,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2278,14 +2495,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -2294,22 +2515,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -2321,8 +2548,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2336,22 +2565,28 @@
         <v>4303</v>
       </c>
       <c r="E4" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G4" s="5">
         <v>3106</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>2245</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>1180</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>718</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
@@ -2365,22 +2600,28 @@
         <v>177</v>
       </c>
       <c r="E5" s="9">
+        <v>186</v>
+      </c>
+      <c r="F5" s="10">
+        <v>177</v>
+      </c>
+      <c r="G5" s="9">
         <v>124</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>87</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>70</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>35</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>36</v>
       </c>
@@ -2394,22 +2635,28 @@
         <v>386</v>
       </c>
       <c r="E6" s="19">
+        <v>314</v>
+      </c>
+      <c r="F6" s="20">
+        <v>386</v>
+      </c>
+      <c r="G6" s="19">
         <v>307</v>
       </c>
-      <c r="F6" s="19">
+      <c r="H6" s="19">
         <v>183</v>
       </c>
-      <c r="G6" s="19">
+      <c r="I6" s="19">
         <v>90</v>
       </c>
-      <c r="H6" s="19">
+      <c r="J6" s="19">
         <v>53</v>
       </c>
-      <c r="I6" s="20">
+      <c r="K6" s="20">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -2423,22 +2670,28 @@
         <v>1146</v>
       </c>
       <c r="E7" s="12">
+        <v>1452</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1146</v>
+      </c>
+      <c r="G7" s="12">
         <v>1010</v>
       </c>
-      <c r="F7" s="12">
+      <c r="H7" s="12">
         <v>722</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>357</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>201</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="17" t="s">
         <v>38</v>
       </c>
@@ -2452,22 +2705,28 @@
         <v>57</v>
       </c>
       <c r="E8" s="19">
+        <v>67</v>
+      </c>
+      <c r="F8" s="20">
+        <v>57</v>
+      </c>
+      <c r="G8" s="19">
         <v>35</v>
       </c>
-      <c r="F8" s="19">
+      <c r="H8" s="19">
         <v>41</v>
       </c>
-      <c r="G8" s="19">
+      <c r="I8" s="19">
         <v>28</v>
       </c>
-      <c r="H8" s="19">
+      <c r="J8" s="19">
         <v>9</v>
       </c>
-      <c r="I8" s="20">
+      <c r="K8" s="20">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -2481,22 +2740,28 @@
         <v>1440</v>
       </c>
       <c r="E9" s="12">
+        <v>1032</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1440</v>
+      </c>
+      <c r="G9" s="12">
         <v>943</v>
       </c>
-      <c r="F9" s="12">
+      <c r="H9" s="12">
         <v>680</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>351</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>225</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>40</v>
       </c>
@@ -2510,22 +2775,28 @@
         <v>80</v>
       </c>
       <c r="E10" s="19">
+        <v>120</v>
+      </c>
+      <c r="F10" s="20">
+        <v>80</v>
+      </c>
+      <c r="G10" s="19">
         <v>59</v>
       </c>
-      <c r="F10" s="19">
+      <c r="H10" s="19">
         <v>48</v>
       </c>
-      <c r="G10" s="19">
+      <c r="I10" s="19">
         <v>32</v>
       </c>
-      <c r="H10" s="19">
+      <c r="J10" s="19">
         <v>19</v>
       </c>
-      <c r="I10" s="20">
+      <c r="K10" s="20">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
@@ -2539,22 +2810,28 @@
         <v>1017</v>
       </c>
       <c r="E11" s="15">
+        <v>781</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1017</v>
+      </c>
+      <c r="G11" s="15">
         <v>628</v>
       </c>
-      <c r="F11" s="15">
+      <c r="H11" s="15">
         <v>484</v>
       </c>
-      <c r="G11" s="15">
+      <c r="I11" s="15">
         <v>252</v>
       </c>
-      <c r="H11" s="15">
+      <c r="J11" s="15">
         <v>176</v>
       </c>
-      <c r="I11" s="16">
+      <c r="K11" s="16">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -2566,8 +2843,10 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="12.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -2581,22 +2860,28 @@
         <v>13</v>
       </c>
       <c r="E13" s="5">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5">
         <v>12</v>
       </c>
-      <c r="F13" s="5">
+      <c r="H13" s="5">
         <v>9</v>
       </c>
-      <c r="G13" s="5">
+      <c r="I13" s="5">
         <v>7</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="6">
+      <c r="K13" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1">
+    <row r="14" spans="1:11" ht="12.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -2609,23 +2894,29 @@
       <c r="D14" s="10">
         <v>1</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="10">
         <v>1</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>43</v>
+      <c r="G14" s="9">
+        <v>1</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="12.75" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>36</v>
       </c>
@@ -2641,20 +2932,26 @@
       <c r="E15" s="19">
         <v>4</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="20">
         <v>4</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="19">
+        <v>4</v>
+      </c>
+      <c r="H15" s="19">
+        <v>4</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="J15" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="K15" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
@@ -2668,22 +2965,28 @@
         <v>4</v>
       </c>
       <c r="E16" s="12">
+        <v>3</v>
+      </c>
+      <c r="F16" s="13">
+        <v>4</v>
+      </c>
+      <c r="G16" s="12">
         <v>1</v>
       </c>
-      <c r="F16" s="12">
+      <c r="H16" s="12">
         <v>2</v>
       </c>
-      <c r="G16" s="12">
+      <c r="I16" s="12">
         <v>3</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="J16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="13">
+      <c r="K16" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1">
+    <row r="17" spans="1:11" ht="12.75" customHeight="1">
       <c r="A17" s="17" t="s">
         <v>38</v>
       </c>
@@ -2699,7 +3002,7 @@
       <c r="E17" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="20" t="s">
         <v>43</v>
       </c>
       <c r="G17" s="19" t="s">
@@ -2708,11 +3011,17 @@
       <c r="H17" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="12.75" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>39</v>
       </c>
@@ -2726,22 +3035,28 @@
         <v>3</v>
       </c>
       <c r="E18" s="12">
+        <v>5</v>
+      </c>
+      <c r="F18" s="13">
+        <v>3</v>
+      </c>
+      <c r="G18" s="12">
         <v>4</v>
       </c>
-      <c r="F18" s="12">
+      <c r="H18" s="12">
         <v>1</v>
       </c>
-      <c r="G18" s="12">
+      <c r="I18" s="12">
         <v>3</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="J18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="K18" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1">
+    <row r="19" spans="1:11" ht="12.75" customHeight="1">
       <c r="A19" s="17" t="s">
         <v>40</v>
       </c>
@@ -2754,23 +3069,29 @@
       <c r="D19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="F19" s="19">
-        <v>1</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="J19" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1">
+      <c r="K19" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="12.75" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>41</v>
       </c>
@@ -2784,22 +3105,28 @@
         <v>1</v>
       </c>
       <c r="E20" s="15">
+        <v>3</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+      <c r="G20" s="15">
         <v>2</v>
       </c>
-      <c r="F20" s="15">
+      <c r="H20" s="15">
         <v>1</v>
       </c>
-      <c r="G20" s="15">
+      <c r="I20" s="15">
         <v>1</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="J20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="K20" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -2811,8 +3138,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="12.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -2826,22 +3155,28 @@
         <v>4303</v>
       </c>
       <c r="E22" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F22" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G22" s="5">
         <v>3106</v>
       </c>
-      <c r="F22" s="5">
+      <c r="H22" s="5">
         <v>2245</v>
       </c>
-      <c r="G22" s="5">
+      <c r="I22" s="5">
         <v>1180</v>
       </c>
-      <c r="H22" s="5">
+      <c r="J22" s="5">
         <v>718</v>
       </c>
-      <c r="I22" s="6">
+      <c r="K22" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1">
+    <row r="23" spans="1:11" ht="12.75" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
@@ -2855,22 +3190,28 @@
         <v>322</v>
       </c>
       <c r="E23" s="9">
+        <v>290</v>
+      </c>
+      <c r="F23" s="10">
+        <v>322</v>
+      </c>
+      <c r="G23" s="9">
         <v>215</v>
       </c>
-      <c r="F23" s="9">
+      <c r="H23" s="9">
         <v>167</v>
       </c>
-      <c r="G23" s="9">
+      <c r="I23" s="9">
         <v>102</v>
       </c>
-      <c r="H23" s="9">
+      <c r="J23" s="9">
         <v>60</v>
       </c>
-      <c r="I23" s="10">
+      <c r="K23" s="10">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1">
+    <row r="24" spans="1:11" ht="12.75" customHeight="1">
       <c r="A24" s="17" t="s">
         <v>36</v>
       </c>
@@ -2884,22 +3225,28 @@
         <v>670</v>
       </c>
       <c r="E24" s="19">
+        <v>575</v>
+      </c>
+      <c r="F24" s="20">
+        <v>670</v>
+      </c>
+      <c r="G24" s="19">
         <v>554</v>
       </c>
-      <c r="F24" s="19">
+      <c r="H24" s="19">
         <v>329</v>
       </c>
-      <c r="G24" s="19">
+      <c r="I24" s="19">
         <v>157</v>
       </c>
-      <c r="H24" s="19">
+      <c r="J24" s="19">
         <v>89</v>
       </c>
-      <c r="I24" s="20">
+      <c r="K24" s="20">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1">
+    <row r="25" spans="1:11" ht="12.75" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>37</v>
       </c>
@@ -2913,22 +3260,28 @@
         <v>1383</v>
       </c>
       <c r="E25" s="12">
+        <v>1319</v>
+      </c>
+      <c r="F25" s="13">
+        <v>1383</v>
+      </c>
+      <c r="G25" s="12">
         <v>1002</v>
       </c>
-      <c r="F25" s="12">
+      <c r="H25" s="12">
         <v>749</v>
       </c>
-      <c r="G25" s="12">
+      <c r="I25" s="12">
         <v>394</v>
       </c>
-      <c r="H25" s="12">
+      <c r="J25" s="12">
         <v>216</v>
       </c>
-      <c r="I25" s="13">
+      <c r="K25" s="13">
         <v>283</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1">
+    <row r="26" spans="1:11" ht="12.75" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>38</v>
       </c>
@@ -2942,22 +3295,28 @@
         <v>26</v>
       </c>
       <c r="E26" s="19">
+        <v>40</v>
+      </c>
+      <c r="F26" s="20">
+        <v>26</v>
+      </c>
+      <c r="G26" s="19">
         <v>22</v>
       </c>
-      <c r="F26" s="19">
+      <c r="H26" s="19">
         <v>21</v>
       </c>
-      <c r="G26" s="19">
+      <c r="I26" s="19">
         <v>10</v>
       </c>
-      <c r="H26" s="19">
+      <c r="J26" s="19">
         <v>6</v>
       </c>
-      <c r="I26" s="20">
+      <c r="K26" s="20">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1">
+    <row r="27" spans="1:11" ht="12.75" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>39</v>
       </c>
@@ -2971,22 +3330,28 @@
         <v>890</v>
       </c>
       <c r="E27" s="12">
+        <v>820</v>
+      </c>
+      <c r="F27" s="13">
+        <v>890</v>
+      </c>
+      <c r="G27" s="12">
         <v>629</v>
       </c>
-      <c r="F27" s="12">
+      <c r="H27" s="12">
         <v>487</v>
       </c>
-      <c r="G27" s="12">
+      <c r="I27" s="12">
         <v>256</v>
       </c>
-      <c r="H27" s="12">
+      <c r="J27" s="12">
         <v>153</v>
       </c>
-      <c r="I27" s="13">
+      <c r="K27" s="13">
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="12.75" customHeight="1">
+    <row r="28" spans="1:11" ht="12.75" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>40</v>
       </c>
@@ -3000,22 +3365,28 @@
         <v>145</v>
       </c>
       <c r="E28" s="19">
+        <v>164</v>
+      </c>
+      <c r="F28" s="20">
+        <v>145</v>
+      </c>
+      <c r="G28" s="19">
         <v>101</v>
       </c>
-      <c r="F28" s="19">
+      <c r="H28" s="19">
         <v>67</v>
       </c>
-      <c r="G28" s="19">
+      <c r="I28" s="19">
         <v>47</v>
       </c>
-      <c r="H28" s="19">
+      <c r="J28" s="19">
         <v>34</v>
       </c>
-      <c r="I28" s="20">
+      <c r="K28" s="20">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1">
+    <row r="29" spans="1:11" ht="12.75" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>41</v>
       </c>
@@ -3029,22 +3400,28 @@
         <v>867</v>
       </c>
       <c r="E29" s="15">
+        <v>744</v>
+      </c>
+      <c r="F29" s="16">
+        <v>867</v>
+      </c>
+      <c r="G29" s="15">
         <v>583</v>
       </c>
-      <c r="F29" s="15">
+      <c r="H29" s="15">
         <v>425</v>
       </c>
-      <c r="G29" s="15">
+      <c r="I29" s="15">
         <v>214</v>
       </c>
-      <c r="H29" s="15">
+      <c r="J29" s="15">
         <v>160</v>
       </c>
-      <c r="I29" s="16">
+      <c r="K29" s="16">
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
@@ -3056,8 +3433,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" ht="12.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>9</v>
       </c>
@@ -3071,22 +3450,28 @@
         <v>13</v>
       </c>
       <c r="E31" s="5">
+        <v>17</v>
+      </c>
+      <c r="F31" s="6">
+        <v>13</v>
+      </c>
+      <c r="G31" s="5">
         <v>12</v>
       </c>
-      <c r="F31" s="5">
+      <c r="H31" s="5">
         <v>9</v>
       </c>
-      <c r="G31" s="5">
+      <c r="I31" s="5">
         <v>7</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="6">
+      <c r="K31" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1">
+    <row r="32" spans="1:11" ht="12.75" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>35</v>
       </c>
@@ -3102,20 +3487,26 @@
       <c r="E32" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="G32" s="9">
-        <v>1</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="9">
+        <v>1</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="12.75" customHeight="1">
+      <c r="K32" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="12.75" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>36</v>
       </c>
@@ -3129,22 +3520,28 @@
         <v>1</v>
       </c>
       <c r="E33" s="19">
+        <v>5</v>
+      </c>
+      <c r="F33" s="20">
+        <v>1</v>
+      </c>
+      <c r="G33" s="19">
         <v>3</v>
       </c>
-      <c r="F33" s="19">
+      <c r="H33" s="19">
         <v>2</v>
       </c>
-      <c r="G33" s="19">
+      <c r="I33" s="19">
         <v>1</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="J33" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I33" s="20" t="s">
+      <c r="K33" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="12.75" customHeight="1">
+    <row r="34" spans="1:11" ht="12.75" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>37</v>
       </c>
@@ -3160,20 +3557,26 @@
       <c r="E34" s="12">
         <v>1</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="13">
+        <v>7</v>
+      </c>
+      <c r="G34" s="12">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12">
         <v>2</v>
       </c>
-      <c r="G34" s="12">
+      <c r="I34" s="12">
         <v>4</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="J34" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="13">
+      <c r="K34" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="12.75" customHeight="1">
+    <row r="35" spans="1:11" ht="12.75" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>38</v>
       </c>
@@ -3189,7 +3592,7 @@
       <c r="E35" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="20" t="s">
         <v>43</v>
       </c>
       <c r="G35" s="19" t="s">
@@ -3198,11 +3601,17 @@
       <c r="H35" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J35" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="12.75" customHeight="1">
       <c r="A36" s="7" t="s">
         <v>39</v>
       </c>
@@ -3216,22 +3625,28 @@
         <v>1</v>
       </c>
       <c r="E36" s="12">
+        <v>5</v>
+      </c>
+      <c r="F36" s="13">
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
         <v>4</v>
       </c>
-      <c r="F36" s="12">
+      <c r="H36" s="12">
         <v>2</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="I36" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="J36" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="K36" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="12.75" customHeight="1">
+    <row r="37" spans="1:11" ht="12.75" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>40</v>
       </c>
@@ -3247,20 +3662,26 @@
       <c r="E37" s="19">
         <v>1</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="20">
         <v>1</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="19">
+        <v>1</v>
+      </c>
+      <c r="H37" s="19">
+        <v>1</v>
+      </c>
+      <c r="I37" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="J37" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I37" s="20" t="s">
+      <c r="K37" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="12.75" customHeight="1">
+    <row r="38" spans="1:11" ht="12.75" customHeight="1">
       <c r="A38" s="7" t="s">
         <v>41</v>
       </c>
@@ -3274,22 +3695,28 @@
         <v>2</v>
       </c>
       <c r="E38" s="15">
+        <v>5</v>
+      </c>
+      <c r="F38" s="16">
+        <v>2</v>
+      </c>
+      <c r="G38" s="15">
         <v>3</v>
       </c>
-      <c r="F38" s="15">
+      <c r="H38" s="15">
         <v>2</v>
       </c>
-      <c r="G38" s="15">
+      <c r="I38" s="15">
         <v>1</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="J38" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="K38" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3301,8 +3728,10 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" ht="12.75" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
@@ -3316,22 +3745,28 @@
         <v>4303</v>
       </c>
       <c r="E40" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F40" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G40" s="5">
         <v>3106</v>
       </c>
-      <c r="F40" s="5">
+      <c r="H40" s="5">
         <v>2245</v>
       </c>
-      <c r="G40" s="5">
+      <c r="I40" s="5">
         <v>1180</v>
       </c>
-      <c r="H40" s="5">
+      <c r="J40" s="5">
         <v>718</v>
       </c>
-      <c r="I40" s="6">
+      <c r="K40" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="12.75" customHeight="1">
+    <row r="41" spans="1:11" ht="12.75" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>35</v>
       </c>
@@ -3345,22 +3780,28 @@
         <v>1497</v>
       </c>
       <c r="E41" s="9">
+        <v>1251</v>
+      </c>
+      <c r="F41" s="10">
+        <v>1497</v>
+      </c>
+      <c r="G41" s="9">
         <v>1050</v>
       </c>
-      <c r="F41" s="9">
+      <c r="H41" s="9">
         <v>786</v>
       </c>
-      <c r="G41" s="9">
+      <c r="I41" s="9">
         <v>393</v>
       </c>
-      <c r="H41" s="9">
+      <c r="J41" s="9">
         <v>239</v>
       </c>
-      <c r="I41" s="10">
+      <c r="K41" s="10">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="12.75" customHeight="1">
+    <row r="42" spans="1:11" ht="12.75" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>36</v>
       </c>
@@ -3374,22 +3815,28 @@
         <v>630</v>
       </c>
       <c r="E42" s="19">
+        <v>497</v>
+      </c>
+      <c r="F42" s="20">
+        <v>630</v>
+      </c>
+      <c r="G42" s="19">
         <v>501</v>
       </c>
-      <c r="F42" s="19">
+      <c r="H42" s="19">
         <v>307</v>
       </c>
-      <c r="G42" s="19">
+      <c r="I42" s="19">
         <v>135</v>
       </c>
-      <c r="H42" s="19">
+      <c r="J42" s="19">
         <v>77</v>
       </c>
-      <c r="I42" s="20">
+      <c r="K42" s="20">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="12.75" customHeight="1">
+    <row r="43" spans="1:11" ht="12.75" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>37</v>
       </c>
@@ -3403,22 +3850,28 @@
         <v>1044</v>
       </c>
       <c r="E43" s="12">
+        <v>1149</v>
+      </c>
+      <c r="F43" s="13">
+        <v>1044</v>
+      </c>
+      <c r="G43" s="12">
         <v>816</v>
       </c>
-      <c r="F43" s="12">
+      <c r="H43" s="12">
         <v>603</v>
       </c>
-      <c r="G43" s="12">
+      <c r="I43" s="12">
         <v>321</v>
       </c>
-      <c r="H43" s="12">
+      <c r="J43" s="12">
         <v>178</v>
       </c>
-      <c r="I43" s="13">
+      <c r="K43" s="13">
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1">
+    <row r="44" spans="1:11" ht="12.75" customHeight="1">
       <c r="A44" s="17" t="s">
         <v>38</v>
       </c>
@@ -3432,22 +3885,28 @@
         <v>12</v>
       </c>
       <c r="E44" s="19">
+        <v>22</v>
+      </c>
+      <c r="F44" s="20">
+        <v>12</v>
+      </c>
+      <c r="G44" s="19">
         <v>14</v>
       </c>
-      <c r="F44" s="19">
+      <c r="H44" s="19">
         <v>12</v>
       </c>
-      <c r="G44" s="19">
+      <c r="I44" s="19">
         <v>4</v>
       </c>
-      <c r="H44" s="19">
+      <c r="J44" s="19">
         <v>1</v>
       </c>
-      <c r="I44" s="20">
+      <c r="K44" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="12.75" customHeight="1">
+    <row r="45" spans="1:11" ht="12.75" customHeight="1">
       <c r="A45" s="7" t="s">
         <v>39</v>
       </c>
@@ -3461,22 +3920,28 @@
         <v>113</v>
       </c>
       <c r="E45" s="12">
+        <v>112</v>
+      </c>
+      <c r="F45" s="13">
+        <v>113</v>
+      </c>
+      <c r="G45" s="12">
         <v>78</v>
       </c>
-      <c r="F45" s="12">
+      <c r="H45" s="12">
         <v>56</v>
       </c>
-      <c r="G45" s="12">
+      <c r="I45" s="12">
         <v>48</v>
       </c>
-      <c r="H45" s="12">
+      <c r="J45" s="12">
         <v>16</v>
       </c>
-      <c r="I45" s="13">
+      <c r="K45" s="13">
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="12.75" customHeight="1">
+    <row r="46" spans="1:11" ht="12.75" customHeight="1">
       <c r="A46" s="17" t="s">
         <v>40</v>
       </c>
@@ -3490,22 +3955,28 @@
         <v>190</v>
       </c>
       <c r="E46" s="19">
+        <v>176</v>
+      </c>
+      <c r="F46" s="20">
+        <v>190</v>
+      </c>
+      <c r="G46" s="19">
         <v>109</v>
       </c>
-      <c r="F46" s="19">
+      <c r="H46" s="19">
         <v>87</v>
       </c>
-      <c r="G46" s="19">
+      <c r="I46" s="19">
         <v>52</v>
       </c>
-      <c r="H46" s="19">
+      <c r="J46" s="19">
         <v>41</v>
       </c>
-      <c r="I46" s="20">
+      <c r="K46" s="20">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="12.75" customHeight="1">
+    <row r="47" spans="1:11" ht="12.75" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>41</v>
       </c>
@@ -3519,22 +3990,28 @@
         <v>817</v>
       </c>
       <c r="E47" s="15">
+        <v>745</v>
+      </c>
+      <c r="F47" s="16">
+        <v>817</v>
+      </c>
+      <c r="G47" s="15">
         <v>538</v>
       </c>
-      <c r="F47" s="15">
+      <c r="H47" s="15">
         <v>394</v>
       </c>
-      <c r="G47" s="15">
+      <c r="I47" s="15">
         <v>227</v>
       </c>
-      <c r="H47" s="15">
+      <c r="J47" s="15">
         <v>166</v>
       </c>
-      <c r="I47" s="16">
+      <c r="K47" s="16">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:11">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -3546,8 +4023,10 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11" ht="12.75" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
@@ -3561,22 +4040,28 @@
         <v>4303</v>
       </c>
       <c r="E49" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F49" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G49" s="5">
         <v>3106</v>
       </c>
-      <c r="F49" s="5">
+      <c r="H49" s="5">
         <v>2245</v>
       </c>
-      <c r="G49" s="5">
+      <c r="I49" s="5">
         <v>1180</v>
       </c>
-      <c r="H49" s="5">
+      <c r="J49" s="5">
         <v>718</v>
       </c>
-      <c r="I49" s="6">
+      <c r="K49" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="12.75" customHeight="1">
+    <row r="50" spans="1:11" ht="12.75" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>35</v>
       </c>
@@ -3590,22 +4075,28 @@
         <v>232</v>
       </c>
       <c r="E50" s="9">
+        <v>205</v>
+      </c>
+      <c r="F50" s="10">
+        <v>232</v>
+      </c>
+      <c r="G50" s="9">
         <v>146</v>
       </c>
-      <c r="F50" s="9">
+      <c r="H50" s="9">
         <v>108</v>
       </c>
-      <c r="G50" s="9">
+      <c r="I50" s="9">
         <v>75</v>
       </c>
-      <c r="H50" s="9">
+      <c r="J50" s="9">
         <v>56</v>
       </c>
-      <c r="I50" s="10">
+      <c r="K50" s="10">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="12.75" customHeight="1">
+    <row r="51" spans="1:11" ht="12.75" customHeight="1">
       <c r="A51" s="17" t="s">
         <v>36</v>
       </c>
@@ -3619,22 +4110,28 @@
         <v>346</v>
       </c>
       <c r="E51" s="19">
+        <v>332</v>
+      </c>
+      <c r="F51" s="20">
+        <v>346</v>
+      </c>
+      <c r="G51" s="19">
         <v>294</v>
       </c>
-      <c r="F51" s="19">
+      <c r="H51" s="19">
         <v>185</v>
       </c>
-      <c r="G51" s="19">
+      <c r="I51" s="19">
         <v>96</v>
       </c>
-      <c r="H51" s="19">
+      <c r="J51" s="19">
         <v>45</v>
       </c>
-      <c r="I51" s="20">
+      <c r="K51" s="20">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="12.75" customHeight="1">
+    <row r="52" spans="1:11" ht="12.75" customHeight="1">
       <c r="A52" s="7" t="s">
         <v>37</v>
       </c>
@@ -3648,22 +4145,28 @@
         <v>1207</v>
       </c>
       <c r="E52" s="12">
+        <v>1309</v>
+      </c>
+      <c r="F52" s="13">
+        <v>1207</v>
+      </c>
+      <c r="G52" s="12">
         <v>1000</v>
       </c>
-      <c r="F52" s="12">
+      <c r="H52" s="12">
         <v>695</v>
       </c>
-      <c r="G52" s="12">
+      <c r="I52" s="12">
         <v>344</v>
       </c>
-      <c r="H52" s="12">
+      <c r="J52" s="12">
         <v>187</v>
       </c>
-      <c r="I52" s="13">
+      <c r="K52" s="13">
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="12.75" customHeight="1">
+    <row r="53" spans="1:11" ht="12.75" customHeight="1">
       <c r="A53" s="17" t="s">
         <v>38</v>
       </c>
@@ -3677,22 +4180,28 @@
         <v>51</v>
       </c>
       <c r="E53" s="19">
+        <v>53</v>
+      </c>
+      <c r="F53" s="20">
+        <v>51</v>
+      </c>
+      <c r="G53" s="19">
         <v>30</v>
       </c>
-      <c r="F53" s="19">
+      <c r="H53" s="19">
         <v>35</v>
       </c>
-      <c r="G53" s="19">
+      <c r="I53" s="19">
         <v>15</v>
       </c>
-      <c r="H53" s="19">
+      <c r="J53" s="19">
         <v>8</v>
       </c>
-      <c r="I53" s="20">
+      <c r="K53" s="20">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="12.75" customHeight="1">
+    <row r="54" spans="1:11" ht="12.75" customHeight="1">
       <c r="A54" s="7" t="s">
         <v>39</v>
       </c>
@@ -3706,22 +4215,28 @@
         <v>1292</v>
       </c>
       <c r="E54" s="12">
+        <v>1002</v>
+      </c>
+      <c r="F54" s="13">
+        <v>1292</v>
+      </c>
+      <c r="G54" s="12">
         <v>863</v>
       </c>
-      <c r="F54" s="12">
+      <c r="H54" s="12">
         <v>653</v>
       </c>
-      <c r="G54" s="12">
+      <c r="I54" s="12">
         <v>330</v>
       </c>
-      <c r="H54" s="12">
+      <c r="J54" s="12">
         <v>197</v>
       </c>
-      <c r="I54" s="13">
+      <c r="K54" s="13">
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="12.75" customHeight="1">
+    <row r="55" spans="1:11" ht="12.75" customHeight="1">
       <c r="A55" s="17" t="s">
         <v>40</v>
       </c>
@@ -3735,22 +4250,28 @@
         <v>86</v>
       </c>
       <c r="E55" s="19">
+        <v>125</v>
+      </c>
+      <c r="F55" s="20">
+        <v>86</v>
+      </c>
+      <c r="G55" s="19">
         <v>61</v>
       </c>
-      <c r="F55" s="19">
+      <c r="H55" s="19">
         <v>51</v>
       </c>
-      <c r="G55" s="19">
+      <c r="I55" s="19">
         <v>31</v>
       </c>
-      <c r="H55" s="19">
+      <c r="J55" s="19">
         <v>25</v>
       </c>
-      <c r="I55" s="20">
+      <c r="K55" s="20">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="12.75" customHeight="1">
+    <row r="56" spans="1:11" ht="12.75" customHeight="1">
       <c r="A56" s="7" t="s">
         <v>41</v>
       </c>
@@ -3764,25 +4285,32 @@
         <v>1089</v>
       </c>
       <c r="E56" s="15">
+        <v>926</v>
+      </c>
+      <c r="F56" s="16">
+        <v>1089</v>
+      </c>
+      <c r="G56" s="15">
         <v>712</v>
       </c>
-      <c r="F56" s="15">
+      <c r="H56" s="15">
         <v>518</v>
       </c>
-      <c r="G56" s="15">
+      <c r="I56" s="15">
         <v>289</v>
       </c>
-      <c r="H56" s="15">
+      <c r="J56" s="15">
         <v>200</v>
       </c>
-      <c r="I56" s="16">
+      <c r="K56" s="16">
         <v>242</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3791,7 +4319,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -3811,9 +4339,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3822,14 +4352,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -3838,22 +4372,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -3865,8 +4405,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -3880,22 +4422,28 @@
         <v>1156</v>
       </c>
       <c r="E4" s="5">
+        <v>1211</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1156</v>
+      </c>
+      <c r="G4" s="5">
         <v>994</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>660</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>319</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>154</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>49</v>
       </c>
@@ -3909,22 +4457,28 @@
         <v>476</v>
       </c>
       <c r="E5" s="9">
+        <v>473</v>
+      </c>
+      <c r="F5" s="10">
+        <v>476</v>
+      </c>
+      <c r="G5" s="9">
         <v>433</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>289</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>102</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>43</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
@@ -3938,22 +4492,28 @@
         <v>104</v>
       </c>
       <c r="E6" s="19">
+        <v>112</v>
+      </c>
+      <c r="F6" s="20">
+        <v>104</v>
+      </c>
+      <c r="G6" s="19">
         <v>97</v>
       </c>
-      <c r="F6" s="19">
+      <c r="H6" s="19">
         <v>55</v>
       </c>
-      <c r="G6" s="19">
+      <c r="I6" s="19">
         <v>25</v>
       </c>
-      <c r="H6" s="19">
+      <c r="J6" s="19">
         <v>18</v>
       </c>
-      <c r="I6" s="20">
+      <c r="K6" s="20">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>51</v>
       </c>
@@ -3967,22 +4527,28 @@
         <v>302</v>
       </c>
       <c r="E7" s="12">
+        <v>293</v>
+      </c>
+      <c r="F7" s="13">
+        <v>302</v>
+      </c>
+      <c r="G7" s="12">
         <v>263</v>
       </c>
-      <c r="F7" s="12">
+      <c r="H7" s="12">
         <v>170</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>72</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>31</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="17" t="s">
         <v>52</v>
       </c>
@@ -3996,22 +4562,28 @@
         <v>463</v>
       </c>
       <c r="E8" s="19">
+        <v>507</v>
+      </c>
+      <c r="F8" s="20">
+        <v>463</v>
+      </c>
+      <c r="G8" s="19">
         <v>413</v>
       </c>
-      <c r="F8" s="19">
+      <c r="H8" s="19">
         <v>250</v>
       </c>
-      <c r="G8" s="19">
+      <c r="I8" s="19">
         <v>139</v>
       </c>
-      <c r="H8" s="19">
+      <c r="J8" s="19">
         <v>70</v>
       </c>
-      <c r="I8" s="20">
+      <c r="K8" s="20">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>53</v>
       </c>
@@ -4025,22 +4597,28 @@
         <v>599</v>
       </c>
       <c r="E9" s="12">
+        <v>636</v>
+      </c>
+      <c r="F9" s="13">
+        <v>599</v>
+      </c>
+      <c r="G9" s="12">
         <v>501</v>
       </c>
-      <c r="F9" s="12">
+      <c r="H9" s="12">
         <v>354</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>162</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>90</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>54</v>
       </c>
@@ -4054,22 +4632,28 @@
         <v>118</v>
       </c>
       <c r="E10" s="19">
+        <v>165</v>
+      </c>
+      <c r="F10" s="20">
+        <v>118</v>
+      </c>
+      <c r="G10" s="19">
         <v>128</v>
       </c>
-      <c r="F10" s="19">
+      <c r="H10" s="19">
         <v>78</v>
       </c>
-      <c r="G10" s="19">
+      <c r="I10" s="19">
         <v>33</v>
       </c>
-      <c r="H10" s="19">
+      <c r="J10" s="19">
         <v>14</v>
       </c>
-      <c r="I10" s="20">
+      <c r="K10" s="20">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>55</v>
       </c>
@@ -4083,25 +4667,32 @@
         <v>23</v>
       </c>
       <c r="E11" s="15">
+        <v>26</v>
+      </c>
+      <c r="F11" s="16">
+        <v>23</v>
+      </c>
+      <c r="G11" s="15">
         <v>15</v>
       </c>
-      <c r="F11" s="15">
+      <c r="H11" s="15">
         <v>19</v>
       </c>
-      <c r="G11" s="15">
+      <c r="I11" s="15">
         <v>10</v>
       </c>
-      <c r="H11" s="15">
+      <c r="J11" s="15">
         <v>3</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4110,7 +4701,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -4130,9 +4721,11 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -4141,14 +4734,18 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -4157,22 +4754,28 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -4184,8 +4787,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -4199,22 +4804,28 @@
         <v>4303</v>
       </c>
       <c r="E4" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4303</v>
+      </c>
+      <c r="G4" s="5">
         <v>3106</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>2245</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>1180</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <v>718</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>829</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>57</v>
       </c>
@@ -4228,22 +4839,28 @@
         <v>1711</v>
       </c>
       <c r="E5" s="9">
+        <v>1289</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1711</v>
+      </c>
+      <c r="G5" s="9">
         <v>1228</v>
       </c>
-      <c r="F5" s="9">
+      <c r="H5" s="9">
         <v>841</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>397</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>240</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="10">
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6" s="17" t="s">
         <v>58</v>
       </c>
@@ -4257,22 +4874,28 @@
         <v>818</v>
       </c>
       <c r="E6" s="19">
+        <v>785</v>
+      </c>
+      <c r="F6" s="20">
+        <v>818</v>
+      </c>
+      <c r="G6" s="19">
         <v>598</v>
       </c>
-      <c r="F6" s="19">
+      <c r="H6" s="19">
         <v>448</v>
       </c>
-      <c r="G6" s="19">
+      <c r="I6" s="19">
         <v>233</v>
       </c>
-      <c r="H6" s="19">
+      <c r="J6" s="19">
         <v>140</v>
       </c>
-      <c r="I6" s="20">
+      <c r="K6" s="20">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
@@ -4286,22 +4909,28 @@
         <v>482</v>
       </c>
       <c r="E7" s="12">
+        <v>379</v>
+      </c>
+      <c r="F7" s="13">
+        <v>482</v>
+      </c>
+      <c r="G7" s="12">
         <v>354</v>
       </c>
-      <c r="F7" s="12">
+      <c r="H7" s="12">
         <v>245</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>108</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>69</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="17" t="s">
         <v>60</v>
       </c>
@@ -4315,22 +4944,28 @@
         <v>1294</v>
       </c>
       <c r="E8" s="19">
+        <v>883</v>
+      </c>
+      <c r="F8" s="20">
+        <v>1294</v>
+      </c>
+      <c r="G8" s="19">
         <v>895</v>
       </c>
-      <c r="F8" s="19">
+      <c r="H8" s="19">
         <v>593</v>
       </c>
-      <c r="G8" s="19">
+      <c r="I8" s="19">
         <v>287</v>
       </c>
-      <c r="H8" s="19">
+      <c r="J8" s="19">
         <v>173</v>
       </c>
-      <c r="I8" s="20">
+      <c r="K8" s="20">
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -4344,22 +4979,28 @@
         <v>195</v>
       </c>
       <c r="E9" s="12">
+        <v>172</v>
+      </c>
+      <c r="F9" s="13">
+        <v>195</v>
+      </c>
+      <c r="G9" s="12">
         <v>159</v>
       </c>
-      <c r="F9" s="12">
+      <c r="H9" s="12">
         <v>102</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>39</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>19</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>41</v>
       </c>
@@ -4373,22 +5014,28 @@
         <v>669</v>
       </c>
       <c r="E10" s="19">
+        <v>689</v>
+      </c>
+      <c r="F10" s="20">
+        <v>669</v>
+      </c>
+      <c r="G10" s="19">
         <v>495</v>
       </c>
-      <c r="F10" s="19">
+      <c r="H10" s="19">
         <v>391</v>
       </c>
-      <c r="G10" s="19">
+      <c r="I10" s="19">
         <v>201</v>
       </c>
-      <c r="H10" s="19">
+      <c r="J10" s="19">
         <v>106</v>
       </c>
-      <c r="I10" s="20">
+      <c r="K10" s="20">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
         <v>61</v>
       </c>
@@ -4402,25 +5049,32 @@
         <v>1420</v>
       </c>
       <c r="E11" s="15">
+        <v>1463</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1420</v>
+      </c>
+      <c r="G11" s="15">
         <v>1003</v>
       </c>
-      <c r="F11" s="15">
+      <c r="H11" s="15">
         <v>740</v>
       </c>
-      <c r="G11" s="15">
+      <c r="I11" s="15">
         <v>424</v>
       </c>
-      <c r="H11" s="15">
+      <c r="J11" s="15">
         <v>281</v>
       </c>
-      <c r="I11" s="16">
+      <c r="K11" s="16">
         <v>369</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fix for freeze loc in chain structures.
</commit_message>
<xml_diff>
--- a/tests/basic.xlsx
+++ b/tests/basic.xlsx
@@ -1147,8 +1147,8 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -1564,8 +1564,8 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -1806,8 +1806,8 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2258,8 +2258,8 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2465,8 +2465,8 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -4322,8 +4322,8 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -4704,8 +4704,8 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
     </sheetView>

</xml_diff>